<commit_message>
Added some new improvement to the code.
</commit_message>
<xml_diff>
--- a/2023-10-01sales.xlsx
+++ b/2023-10-01sales.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="14">
   <si>
     <t>PC</t>
   </si>
@@ -31,37 +31,31 @@
     <t>QTY</t>
   </si>
   <si>
-    <t>121211</t>
-  </si>
-  <si>
-    <t>2023-10-27</t>
-  </si>
-  <si>
-    <t>Caro White Soap</t>
+    <t>121212</t>
+  </si>
+  <si>
+    <t>2023-10-30</t>
+  </si>
+  <si>
+    <t>Caro White Cream</t>
+  </si>
+  <si>
+    <t>1800</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>121210</t>
+  </si>
+  <si>
+    <t>Oral B</t>
   </si>
   <si>
     <t>800</t>
   </si>
   <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>121212</t>
-  </si>
-  <si>
-    <t>Caro White Cream</t>
-  </si>
-  <si>
-    <t>1800</t>
-  </si>
-  <si>
-    <t>121210</t>
-  </si>
-  <si>
-    <t>Oral B</t>
-  </si>
-  <si>
-    <t>2023-10-28</t>
+    <t>2023-10-31</t>
   </si>
 </sst>
 </file>
@@ -393,7 +387,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -435,16 +429,16 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B3" t="s">
         <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D3" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E3" t="s">
         <v>9</v>
@@ -469,16 +463,16 @@
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="C5" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D5" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E5" t="s">
         <v>9</v>
@@ -486,86 +480,18 @@
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
         <v>13</v>
       </c>
-      <c r="B6" t="s">
-        <v>6</v>
-      </c>
       <c r="C6" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="D6" t="s">
         <v>8</v>
       </c>
       <c r="E6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7" t="s">
-        <v>11</v>
-      </c>
-      <c r="D7" t="s">
-        <v>12</v>
-      </c>
-      <c r="E7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="A8" t="s">
-        <v>10</v>
-      </c>
-      <c r="B8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C8" t="s">
-        <v>11</v>
-      </c>
-      <c r="D8" t="s">
-        <v>12</v>
-      </c>
-      <c r="E8" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="A9" t="s">
-        <v>5</v>
-      </c>
-      <c r="B9" t="s">
-        <v>15</v>
-      </c>
-      <c r="C9" t="s">
-        <v>7</v>
-      </c>
-      <c r="D9" t="s">
-        <v>8</v>
-      </c>
-      <c r="E9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
-      <c r="A10" t="s">
-        <v>10</v>
-      </c>
-      <c r="B10" t="s">
-        <v>15</v>
-      </c>
-      <c r="C10" t="s">
-        <v>11</v>
-      </c>
-      <c r="D10" t="s">
-        <v>12</v>
-      </c>
-      <c r="E10" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
More improvement added to the code.
</commit_message>
<xml_diff>
--- a/2023-10-01sales.xlsx
+++ b/2023-10-01sales.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="14">
   <si>
     <t>PC</t>
   </si>
@@ -387,7 +387,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -495,6 +495,40 @@
         <v>9</v>
       </c>
     </row>
+    <row r="7" spans="1:5">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" t="s">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>